<commit_message>
SW: Bugfix; FW: Bugfix - all but sensor fully functioning
FW: critical bug catched by entrance, probably from loggia HVAC
</commit_message>
<xml_diff>
--- a/DOCS/Notes/heater_PWM_on_load.xlsx
+++ b/DOCS/Notes/heater_PWM_on_load.xlsx
@@ -91,83 +91,238 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$B$25</c:f>
+              <c:f>Sheet1!$B$5:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="15">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="16">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="17">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="18">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="19">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="23">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="24">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="25">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$C$25</c:f>
+              <c:f>Sheet1!$D$5:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.87</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>10.55</c:v>
                 </c:pt>
@@ -181,51 +336,66 @@
                   <c:v>10.06</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>9.98</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>9.44</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>8.82</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
+                  <c:v>7.97</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>7.7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>6.93</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>5.99</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>5.56</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>4.8899999999999997</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>4.0999999999999996</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>3.58</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>2.75</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>2.21</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>1.7</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="21">
                   <c:v>1.18</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="22">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="23">
                   <c:v>0.62</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="24">
                   <c:v>0.16</c:v>
                 </c:pt>
               </c:numCache>
@@ -241,11 +411,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="55414144"/>
-        <c:axId val="55414720"/>
+        <c:axId val="137819200"/>
+        <c:axId val="127263296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55414144"/>
+        <c:axId val="137819200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -256,12 +426,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55414720"/>
+        <c:crossAx val="127263296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55414720"/>
+        <c:axId val="127263296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -272,7 +442,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55414144"/>
+        <c:crossAx val="137819200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -298,16 +468,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>90073</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>48660</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>105395</xdr:rowOff>
+      <xdr:rowOff>6003</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>438978</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>181595</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>397565</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>82203</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -616,28 +786,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G29"/>
+  <dimension ref="B2:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C5">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>127</v>
       </c>
@@ -645,7 +818,7 @@
         <v>10.55</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>120</v>
       </c>
@@ -653,7 +826,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>110</v>
       </c>
@@ -661,201 +834,274 @@
         <v>10.37</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>90</v>
       </c>
       <c r="C9">
         <v>10.06</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10">
+        <v>86</v>
+      </c>
+      <c r="C10">
+        <v>9.98</v>
+      </c>
+      <c r="D10">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11">
         <v>70</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>9.44</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12">
         <v>60</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>8.82</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>52</v>
+      </c>
+      <c r="C13">
+        <v>7.97</v>
+      </c>
+      <c r="D13">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14">
         <v>50</v>
       </c>
-      <c r="C12">
+      <c r="C14">
         <v>7.7</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15">
         <v>45</v>
       </c>
-      <c r="C13">
+      <c r="C15">
         <v>6.93</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>40</v>
-      </c>
-      <c r="C14">
-        <v>5.99</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>38</v>
-      </c>
-      <c r="C15">
-        <v>5.56</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C16">
-        <v>4.8899999999999997</v>
+        <v>6.9</v>
+      </c>
+      <c r="D16">
+        <v>6.87</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C17">
-        <v>4.0999999999999996</v>
+        <v>5.99</v>
+      </c>
+      <c r="D17">
+        <v>6.9</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C18">
-        <v>3.58</v>
+        <v>5.56</v>
+      </c>
+      <c r="D18">
+        <v>5.6</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C19">
-        <v>2.75</v>
+        <v>4.8899999999999997</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C20">
-        <v>2.21</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C21">
-        <v>1.7</v>
+        <v>3.58</v>
+      </c>
+      <c r="D21">
+        <v>3.6</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C22">
-        <v>1.18</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C24">
-        <v>0.62</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
+        <v>1.9</v>
+      </c>
+      <c r="D24">
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C25">
-        <v>0.16</v>
-      </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-      <c r="F25">
         <v>1.9</v>
       </c>
-      <c r="G25">
-        <v>24</v>
+      <c r="D25">
+        <v>1.95</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>21</v>
+      </c>
+      <c r="C27">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>20</v>
+      </c>
+      <c r="C28">
         <v>1</v>
       </c>
-      <c r="C26">
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>18</v>
+      </c>
+      <c r="C29">
+        <v>0.62</v>
+      </c>
+      <c r="E29">
         <v>0</v>
       </c>
-      <c r="E26">
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>15</v>
+      </c>
+      <c r="C30">
+        <v>0.16</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>1.9</v>
+      </c>
+      <c r="G30">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
         <v>4</v>
       </c>
-      <c r="F26">
+      <c r="F31">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G26">
+      <c r="G31">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E27">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E32">
         <v>6</v>
       </c>
-      <c r="F27">
+      <c r="F32">
         <v>5.96</v>
       </c>
-      <c r="G27">
+      <c r="G32">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E28">
+    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E33">
         <v>8</v>
       </c>
-      <c r="F28">
+      <c r="F33">
         <v>7.97</v>
       </c>
-      <c r="G28">
+      <c r="G33">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E29">
+    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E34">
         <v>10</v>
       </c>
-      <c r="F29">
+      <c r="F34">
         <v>9.98</v>
       </c>
-      <c r="G29">
+      <c r="G34">
         <v>86</v>
       </c>
     </row>

</xml_diff>